<commit_message>
Timesheets all up to date. That's about it all wrapped up. +20 hours the dream.
</commit_message>
<xml_diff>
--- a/man/completed sheets/2016-02-08/Oliver Earl.xlsx
+++ b/man/completed sheets/2016-02-08/Oliver Earl.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -68,6 +68,30 @@
   </si>
   <si>
     <t>No problems completing this apart from the tedium required</t>
+  </si>
+  <si>
+    <t>SE_05_QA_01/02/03/04</t>
+  </si>
+  <si>
+    <t>Documentation QA</t>
+  </si>
+  <si>
+    <t>Final QA for document handover</t>
+  </si>
+  <si>
+    <t>Extensive QA of all documents, including testing and document specification.</t>
+  </si>
+  <si>
+    <t>SE_05_QA_01/02/03/05</t>
+  </si>
+  <si>
+    <t>Updating Design Spec</t>
+  </si>
+  <si>
+    <t>Updating design spec to closer match current system</t>
+  </si>
+  <si>
+    <t>Extensive modification of design spec. This includes the drawing of new diagrams, editing of existing ones, new UI sketches and various additions to improve our design overall.</t>
   </si>
 </sst>
 </file>
@@ -468,7 +492,7 @@
       <pane xSplit="8" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,11 +528,11 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>"Total hours accounted this week: " &amp;TEXT(I1, "hh:mm")</f>
-        <v>Total hours accounted this week: 05:00</v>
+        <v>Total hours accounted this week: 01:00</v>
       </c>
       <c r="I1" s="6">
         <f>SUM(F3:F100)</f>
-        <v>0.20833333333333334</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -571,25 +595,57 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="9"/>
+    <row r="4" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="10">
+        <v>42415</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="10">
+        <v>42415</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G5" s="11">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>

</xml_diff>